<commit_message>
updated lalashan (fixed traits)
</commit_message>
<xml_diff>
--- a/data/lalashan.xlsx
+++ b/data/lalashan.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="lalashan spe" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="lalashan spnames" sheetId="4" r:id="rId4"/>
     <sheet name="lalashan spe all" sheetId="5" r:id="rId5"/>
     <sheet name="lalashan traits all" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="8" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -1661,7 +1662,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1691,6 +1692,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="136"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1715,7 +1724,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1724,6 +1733,7 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2007,7 +2017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CN19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="CN1" sqref="CN1"/>
     </sheetView>
   </sheetViews>
@@ -9584,13 +9594,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I1" sqref="I1:K1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="2" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="13" style="2" bestFit="1" customWidth="1"/>
@@ -12044,8 +12054,8 @@
       <c r="B54" s="2">
         <v>1407.049</v>
       </c>
-      <c r="C54" s="2">
-        <v>1332.3535000000002</v>
+      <c r="C54" s="4">
+        <v>509.66399999999999</v>
       </c>
       <c r="D54" s="2">
         <v>11.138999999999999</v>
@@ -33954,4 +33964,16 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>